<commit_message>
update work to windows
</commit_message>
<xml_diff>
--- a/ds/Project 2/materials/Timetable.xlsx
+++ b/ds/Project 2/materials/Timetable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Line 1" sheetId="1" r:id="rId1"/>
@@ -596,9 +596,6 @@
     <t>小南门</t>
   </si>
   <si>
-    <t>陆家浜</t>
-  </si>
-  <si>
     <t>马当路</t>
   </si>
   <si>
@@ -931,6 +928,10 @@
   </si>
   <si>
     <t>上海火车站</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>陆家浜路</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1570,10 +1571,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>296</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -1822,22 +1823,22 @@
         <v>58</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C1" s="43"/>
     </row>
     <row r="2" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A2" s="43"/>
       <c r="B2" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>208</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="4">
         <v>0.91319444444444453</v>
@@ -1848,7 +1849,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" s="2">
         <v>0.91388888888888886</v>
@@ -1859,7 +1860,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5" s="4">
         <v>0.91527777777777775</v>
@@ -1870,7 +1871,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" s="2">
         <v>0.91736111111111107</v>
@@ -1881,7 +1882,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B7" s="4">
         <v>0.91875000000000007</v>
@@ -1892,7 +1893,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B8" s="2">
         <v>0.92013888888888884</v>
@@ -1903,7 +1904,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B9" s="4">
         <v>0.92152777777777783</v>
@@ -1925,7 +1926,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B11" s="4">
         <v>0.9243055555555556</v>
@@ -1947,7 +1948,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B13" s="4">
         <v>0.9277777777777777</v>
@@ -1958,7 +1959,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B14" s="2">
         <v>0.9291666666666667</v>
@@ -1980,7 +1981,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B16" s="2">
         <v>0.93263888888888891</v>
@@ -2002,7 +2003,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B18" s="2">
         <v>0.93611111111111101</v>
@@ -2024,7 +2025,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B20" s="2">
         <v>0.93958333333333333</v>
@@ -2035,7 +2036,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B21" s="4">
         <v>0.94166666666666676</v>
@@ -2057,7 +2058,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B23" s="4">
         <v>0.94444444444444453</v>
@@ -2068,7 +2069,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B24" s="2">
         <v>0.94652777777777775</v>
@@ -2079,7 +2080,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B25" s="4">
         <v>0.94791666666666663</v>
@@ -2090,7 +2091,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B26" s="2">
         <v>0.94930555555555562</v>
@@ -2101,7 +2102,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>1</v>
@@ -2112,7 +2113,7 @@
     </row>
     <row r="28" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>1</v>
@@ -2123,7 +2124,7 @@
     </row>
     <row r="29" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>1</v>
@@ -2145,7 +2146,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B31" s="4">
         <v>0.95208333333333339</v>
@@ -2156,7 +2157,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B32" s="2">
         <v>0.95347222222222217</v>
@@ -2167,7 +2168,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B33" s="25">
         <v>0.9555555555555556</v>
@@ -2202,22 +2203,22 @@
         <v>58</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C1" s="44"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="44"/>
       <c r="B2" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>234</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B3" s="2">
         <v>0.9375</v>
@@ -2228,7 +2229,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B4" s="4">
         <v>0.93958333333333333</v>
@@ -2239,7 +2240,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B5" s="2">
         <v>0.94305555555555554</v>
@@ -2250,7 +2251,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B6" s="4">
         <v>0.94513888888888886</v>
@@ -2261,7 +2262,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B7" s="2">
         <v>0.94652777777777775</v>
@@ -2272,7 +2273,7 @@
     </row>
     <row r="8" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B8" s="4">
         <v>0.95000000000000007</v>
@@ -2283,7 +2284,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B9" s="2">
         <v>0.95208333333333339</v>
@@ -2294,7 +2295,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B10" s="4">
         <v>0.95347222222222217</v>
@@ -2305,7 +2306,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B11" s="2">
         <v>0.95486111111111116</v>
@@ -2316,7 +2317,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12" s="4">
         <v>0.95694444444444438</v>
@@ -2338,7 +2339,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B14" s="4">
         <v>0.96111111111111114</v>
@@ -2360,7 +2361,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B16" s="4">
         <v>0.96527777777777779</v>
@@ -2382,7 +2383,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B18" s="4">
         <v>0.96805555555555556</v>
@@ -2393,7 +2394,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B19" s="2">
         <v>0.96944444444444444</v>
@@ -2404,7 +2405,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B20" s="4">
         <v>0.97152777777777777</v>
@@ -2415,7 +2416,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B21" s="2">
         <v>0.97291666666666676</v>
@@ -2426,7 +2427,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B22" s="4">
         <v>0.97499999999999998</v>
@@ -2437,7 +2438,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B23" s="2">
         <v>0.97638888888888886</v>
@@ -2448,7 +2449,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B24" s="4">
         <v>0.97777777777777775</v>
@@ -2459,7 +2460,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B25" s="2">
         <v>0.98055555555555562</v>
@@ -2470,7 +2471,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B26" s="4">
         <v>0.98472222222222217</v>
@@ -2481,7 +2482,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B27" s="2">
         <v>0.9868055555555556</v>
@@ -2492,7 +2493,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B28" s="4">
         <v>0.98888888888888893</v>
@@ -2503,7 +2504,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B29" s="2">
         <v>0.9916666666666667</v>
@@ -2514,7 +2515,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B30" s="25">
         <v>0.99305555555555547</v>
@@ -2525,7 +2526,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>1</v>
@@ -2536,7 +2537,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>1</v>
@@ -2547,7 +2548,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>1</v>
@@ -2558,7 +2559,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>1</v>
@@ -2569,7 +2570,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>1</v>
@@ -2580,7 +2581,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>1</v>
@@ -2591,7 +2592,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>1</v>
@@ -2622,15 +2623,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="37">
         <v>0.91666666666666663</v>
@@ -2638,7 +2639,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B3" s="20">
         <v>0.9194444444444444</v>
@@ -2646,7 +2647,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B4" s="19">
         <v>0.92083333333333339</v>
@@ -2654,7 +2655,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B5" s="20">
         <v>0.92222222222222217</v>
@@ -2670,7 +2671,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B7" s="20">
         <v>0.92569444444444438</v>
@@ -2678,7 +2679,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B8" s="19">
         <v>0.9277777777777777</v>
@@ -2686,7 +2687,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B9" s="20">
         <v>0.9291666666666667</v>
@@ -2694,7 +2695,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B10" s="19">
         <v>0.93055555555555547</v>
@@ -2702,7 +2703,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B11" s="20">
         <v>0.93263888888888891</v>
@@ -2710,7 +2711,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B12" s="19">
         <v>0.93402777777777779</v>
@@ -2726,7 +2727,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B14" s="19">
         <v>0.93680555555555556</v>
@@ -2734,7 +2735,7 @@
     </row>
     <row r="15" spans="1:2" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B15" s="20">
         <v>0.93819444444444444</v>
@@ -2742,7 +2743,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B16" s="19">
         <v>0.94097222222222221</v>
@@ -2777,12 +2778,12 @@
         <v>58</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B2" s="25">
         <v>0.9243055555555556</v>
@@ -2790,7 +2791,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B3" s="2">
         <v>0.92569444444444438</v>
@@ -2798,7 +2799,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B4" s="4">
         <v>0.92847222222222225</v>
@@ -2806,7 +2807,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B5" s="2">
         <v>0.93055555555555547</v>
@@ -2814,7 +2815,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B6" s="4">
         <v>0.93194444444444446</v>
@@ -2822,7 +2823,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B7" s="2">
         <v>0.93402777777777779</v>
@@ -2854,15 +2855,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="40" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B2" s="37">
         <v>0.91666666666666663</v>
@@ -2870,7 +2871,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B3" s="20">
         <v>0.91875000000000007</v>
@@ -2878,7 +2879,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B4" s="19">
         <v>0.92291666666666661</v>
@@ -2886,7 +2887,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="22" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B5" s="20">
         <v>0.92986111111111114</v>
@@ -2894,7 +2895,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B6" s="19">
         <v>0.93333333333333324</v>
@@ -2902,7 +2903,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B7" s="20">
         <v>0.93888888888888899</v>
@@ -2910,7 +2911,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B8" s="19">
         <v>0.94374999999999998</v>
@@ -2918,7 +2919,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B9" s="20">
         <v>0.94791666666666663</v>
@@ -2926,7 +2927,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B10" s="19">
         <v>0.9506944444444444</v>
@@ -2934,7 +2935,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B11" s="20">
         <v>0.95486111111111116</v>
@@ -2942,7 +2943,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="39" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B12" s="19">
         <v>0.9590277777777777</v>
@@ -2973,7 +2974,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="22.5" x14ac:dyDescent="0.15">
@@ -3268,8 +3269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3279,7 +3280,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -3380,7 +3381,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B14" s="23">
         <v>0.95694444444444438</v>
@@ -3536,7 +3537,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -3769,7 +3770,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -3881,7 +3882,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -4129,7 +4130,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -4406,8 +4407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4417,7 +4418,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -4671,7 +4672,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4681,7 +4682,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -4718,7 +4719,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
-        <v>189</v>
+        <v>299</v>
       </c>
       <c r="B6" s="4">
         <v>0.94652777777777775</v>
@@ -4726,7 +4727,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" s="2">
         <v>0.94791666666666663</v>
@@ -4734,7 +4735,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8" s="4">
         <v>0.94930555555555562</v>
@@ -4742,7 +4743,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" s="2">
         <v>0.9506944444444444</v>
@@ -4774,7 +4775,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B13" s="2">
         <v>0.95833333333333337</v>
@@ -4782,7 +4783,7 @@
     </row>
     <row r="14" spans="1:2" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B14" s="4">
         <v>0.9604166666666667</v>
@@ -4790,7 +4791,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B15" s="2">
         <v>0.96180555555555547</v>
@@ -4798,7 +4799,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B16" s="4">
         <v>0.96388888888888891</v>
@@ -4806,7 +4807,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B17" s="2">
         <v>0.96597222222222223</v>
@@ -4814,7 +4815,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B18" s="4">
         <v>0.96805555555555556</v>
@@ -4822,7 +4823,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B19" s="2">
         <v>0.97083333333333333</v>
@@ -4830,7 +4831,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B20" s="4">
         <v>0.97499999999999998</v>
@@ -4838,7 +4839,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B21" s="2">
         <v>0.9784722222222223</v>
@@ -4846,7 +4847,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B22" s="4">
         <v>0.98055555555555562</v>
@@ -4854,7 +4855,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" s="2">
         <v>0.98333333333333339</v>
@@ -4862,7 +4863,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" s="4">
         <v>0.98611111111111116</v>
@@ -4870,7 +4871,7 @@
     </row>
     <row r="25" spans="1:2" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B25" s="4">
         <v>0.98819444444444438</v>
@@ -4878,7 +4879,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B26" s="4">
         <v>0.9902777777777777</v>
@@ -4886,7 +4887,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B27" s="25">
         <v>0.99305555555555547</v>

</xml_diff>